<commit_message>
Add county rollup check to excel doc
</commit_message>
<xml_diff>
--- a/Quality Control Checks.xlsx
+++ b/Quality Control Checks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Documents\Code\COVID19\quality-control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinboehmer/Repos/covid-tracking/quality-control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32F5615-CA9C-4483-B574-F19BCE472798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4FBCFC-155B-C841-8F4A-BD4B9FAEF25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{57F22620-3E69-423A-AD47-BBE5DB20F76E}"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="15800" activeTab="3" xr2:uid="{57F22620-3E69-423A-AD47-BBE5DB20F76E}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="160">
   <si>
     <t>Name</t>
   </si>
@@ -359,18 +359,9 @@
     <t>2. Use them to form an expected range</t>
   </si>
   <si>
-    <t>For the lower bound -- use 90% of linear result.</t>
-  </si>
-  <si>
-    <t>For the upper bound -- use 110% of exponent result</t>
-  </si>
-  <si>
     <t>3. This will replace the static thresholds we currently have</t>
   </si>
   <si>
-    <t>Note -- we expect to the change the model in the future but it works against existing history</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
@@ -440,9 +431,6 @@
     <t>too vague to implement</t>
   </si>
   <si>
-    <t>need data source</t>
-  </si>
-  <si>
     <t>incomplete request</t>
   </si>
   <si>
@@ -486,6 +474,48 @@
   </si>
   <si>
     <t>README</t>
+  </si>
+  <si>
+    <t>expected_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enabled </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   For the lower bound -- use 90% of linear result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   For the upper bound -- use 110% of exponent result</t>
+  </si>
+  <si>
+    <t>Note -- we expect to the change the exp model in the future but it works against existing history</t>
+  </si>
+  <si>
+    <t>counties_rollup_to_state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positive, death, recovered (worksheet only) </t>
+  </si>
+  <si>
+    <t>Pulls latest day's data from NYT, CSBS, and CDS county datasets</t>
+  </si>
+  <si>
+    <t>Uses the min and max of positives, deaths, recovered from the datasets</t>
+  </si>
+  <si>
+    <t>to set a range of "acceptable" values for the state aggregate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ie min(nyt_positives, cds_positives, csbs_positives) = lower bound for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   acceptable state positives count</t>
+  </si>
+  <si>
+    <t>If the state positive count falls outside of the (min, max) county aggregate</t>
+  </si>
+  <si>
+    <t>range, it throws an error</t>
   </si>
 </sst>
 </file>
@@ -629,7 +659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -648,6 +678,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -965,43 +996,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5A4458-58B7-48A9-92A8-DD5DDACD513E}">
   <dimension ref="A3:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.9296875" customWidth="1"/>
-    <col min="3" max="3" width="15.53125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -1009,7 +1040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
@@ -1017,7 +1048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>31</v>
       </c>
@@ -1028,7 +1059,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>18</v>
       </c>
@@ -1039,7 +1070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
@@ -1050,7 +1081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>21</v>
       </c>
@@ -1061,7 +1092,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>23</v>
       </c>
@@ -1072,7 +1103,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>25</v>
       </c>
@@ -1083,7 +1114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>27</v>
       </c>
@@ -1094,7 +1125,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>29</v>
       </c>
@@ -1102,12 +1133,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1115,7 +1146,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1123,7 +1154,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1131,7 +1162,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1139,7 +1170,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1147,7 +1178,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1155,7 +1186,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>7</v>
       </c>
@@ -1166,7 +1197,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>8</v>
       </c>
@@ -1174,12 +1205,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>9</v>
       </c>
@@ -1187,7 +1218,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>51</v>
       </c>
@@ -1199,27 +1230,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB76AACD-064E-44C8-8A43-FF686AF1BB13}">
-  <dimension ref="B3:F42"/>
+  <dimension ref="B3:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="53.19921875" customWidth="1"/>
-    <col min="6" max="6" width="80.06640625" customWidth="1"/>
+    <col min="5" max="5" width="53.1640625" customWidth="1"/>
+    <col min="6" max="6" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:6" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1267,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
@@ -1251,7 +1282,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>54</v>
       </c>
@@ -1268,7 +1299,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>2</v>
       </c>
@@ -1285,7 +1316,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -1302,7 +1333,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>66</v>
       </c>
@@ -1310,7 +1341,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1319,7 +1350,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1333,7 +1364,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D14" s="10" t="s">
         <v>89</v>
       </c>
@@ -1341,7 +1372,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D15" s="10" t="s">
         <v>90</v>
       </c>
@@ -1352,7 +1383,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1361,7 +1392,7 @@
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -1375,12 +1406,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1391,7 +1422,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -1405,7 +1436,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1414,7 +1445,7 @@
       </c>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>7</v>
       </c>
@@ -1429,7 +1460,7 @@
       </c>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -1443,7 +1474,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1452,7 +1483,7 @@
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
@@ -1469,12 +1500,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>94</v>
       </c>
@@ -1482,27 +1513,27 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E35" s="15" t="s">
         <v>98</v>
       </c>
@@ -1510,64 +1541,168 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E36" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C38" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D39">
         <v>100</v>
       </c>
       <c r="E39" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.45">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D40">
         <v>900</v>
       </c>
       <c r="E40" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D41">
         <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="18"/>
+      <c r="C42" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="18">
         <v>1000</v>
       </c>
-      <c r="E42" t="s">
-        <v>116</v>
+      <c r="E42" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" t="s">
+        <v>152</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E55" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E56" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E57" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E58" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E59" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E60" s="10" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1577,52 +1712,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67B930F-F2B6-4280-910B-7201BACFCFCD}">
-  <dimension ref="B3:C13"/>
+  <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:3" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:2" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1635,145 +1735,145 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.06640625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="C9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B7" s="5" t="s">
+      <c r="C10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="5" t="s">
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
+      <c r="C23" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>140</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" t="s">
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B25" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make county test more forgiving of differences
</commit_message>
<xml_diff>
--- a/Quality Control Checks.xlsx
+++ b/Quality Control Checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinboehmer/Repos/covid-tracking/quality-control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4FBCFC-155B-C841-8F4A-BD4B9FAEF25F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3AE0CE-31F7-3241-979D-2A048C71DF07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="15800" activeTab="3" xr2:uid="{57F22620-3E69-423A-AD47-BBE5DB20F76E}"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="15800" activeTab="1" xr2:uid="{57F22620-3E69-423A-AD47-BBE5DB20F76E}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="159">
   <si>
     <t>Name</t>
   </si>
@@ -494,28 +494,25 @@
     <t>counties_rollup_to_state</t>
   </si>
   <si>
-    <t xml:space="preserve">positive, death, recovered (worksheet only) </t>
-  </si>
-  <si>
     <t>Pulls latest day's data from NYT, CSBS, and CDS county datasets</t>
   </si>
   <si>
-    <t>Uses the min and max of positives, deaths, recovered from the datasets</t>
-  </si>
-  <si>
-    <t>to set a range of "acceptable" values for the state aggregate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   ie min(nyt_positives, cds_positives, csbs_positives) = lower bound for</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   acceptable state positives count</t>
-  </si>
-  <si>
-    <t>If the state positive count falls outside of the (min, max) county aggregate</t>
-  </si>
-  <si>
-    <t>range, it throws an error</t>
+    <t>positive, death</t>
+  </si>
+  <si>
+    <t>Chooses whichever county aggregate of positives and deaths matches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">covid-tracking numbers most closely. Computes the error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(max-min)/covid_tracking_state_totals. Current acceptance thresholds </t>
+  </si>
+  <si>
+    <t>set to .1 for positive test count and .2 for death count (which is more</t>
+  </si>
+  <si>
+    <t>error prone)</t>
   </si>
 </sst>
 </file>
@@ -1232,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB76AACD-064E-44C8-8A43-FF686AF1BB13}">
   <dimension ref="B3:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1669,10 +1666,10 @@
         <v>56</v>
       </c>
       <c r="D54" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.2">
@@ -1701,9 +1698,7 @@
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E60" s="10" t="s">
-        <v>159</v>
-      </c>
+      <c r="E60" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1735,8 +1730,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>